<commit_message>
Unidad 1 Practica 7 finalizada
</commit_message>
<xml_diff>
--- a/Unidad 1/U1_Experimentos.xlsx
+++ b/Unidad 1/U1_Experimentos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21540" windowHeight="9540" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21540" windowHeight="9540" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="U1_P2_1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="U1_P4_1" sheetId="4" r:id="rId4"/>
     <sheet name="U1_P5_1" sheetId="5" r:id="rId5"/>
     <sheet name="U1_P6_1" sheetId="6" r:id="rId6"/>
+    <sheet name="U1_P7_1" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_Toc524866089" localSheetId="0">U1_P2_1!$G$33</definedName>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="95">
   <si>
     <t>Coordenadas:</t>
   </si>
@@ -293,6 +294,33 @@
   </si>
   <si>
     <t>Desvacion estandar</t>
+  </si>
+  <si>
+    <t>Vector</t>
+  </si>
+  <si>
+    <t>Matriz</t>
+  </si>
+  <si>
+    <t>Suma:</t>
+  </si>
+  <si>
+    <t>Media:</t>
+  </si>
+  <si>
+    <t>Moda:</t>
+  </si>
+  <si>
+    <t>Varianza:</t>
+  </si>
+  <si>
+    <t>Menor:</t>
+  </si>
+  <si>
+    <t>Mayor:</t>
+  </si>
+  <si>
+    <t>=</t>
   </si>
 </sst>
 </file>
@@ -488,7 +516,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -567,6 +595,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
@@ -888,22 +925,22 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="24" t="s">
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="26"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="2">
         <v>1</v>
       </c>
@@ -919,7 +956,7 @@
       <c r="G2" s="2">
         <v>5</v>
       </c>
-      <c r="H2" s="24"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1060,21 +1097,21 @@
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="J8" s="24" t="s">
+      <c r="J8" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="25" t="s">
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="29" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1082,18 +1119,18 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
       <c r="J9" s="4" t="s">
         <v>26</v>
       </c>
@@ -1103,15 +1140,15 @@
       <c r="L9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="M9" s="25"/>
+      <c r="M9" s="29"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="26"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="27"/>
       <c r="G10" s="2">
         <v>1</v>
       </c>
@@ -1303,14 +1340,14 @@
       </c>
     </row>
     <row r="17" spans="2:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="24" t="s">
+      <c r="C17" s="27"/>
+      <c r="D17" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="28" t="s">
         <v>19</v>
       </c>
       <c r="G17" s="2">
@@ -1342,8 +1379,8 @@
       <c r="C18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
       <c r="G18" s="2">
         <v>9</v>
       </c>
@@ -1831,6 +1868,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="H1:H2"/>
@@ -1839,12 +1882,6 @@
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1855,7 +1892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView topLeftCell="K13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="K19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F24" sqref="F24:S28"/>
     </sheetView>
   </sheetViews>
@@ -2085,28 +2122,28 @@
       <c r="A15" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="29" t="s">
+      <c r="G15" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="31" t="s">
+      <c r="H15" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="I15" s="33" t="s">
+      <c r="I15" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="33"/>
-      <c r="O15" s="33"/>
-      <c r="P15" s="33"/>
-      <c r="Q15" s="33"/>
-      <c r="R15" s="33"/>
-      <c r="S15" s="33"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="36"/>
+      <c r="R15" s="36"/>
+      <c r="S15" s="36"/>
       <c r="T15" s="5" t="s">
         <v>31</v>
       </c>
@@ -2115,9 +2152,9 @@
       <c r="A16" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="32"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="35"/>
       <c r="I16" s="7" t="s">
         <v>51</v>
       </c>
@@ -2443,34 +2480,34 @@
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F24" s="24" t="s">
+      <c r="F24" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="24" t="s">
+      <c r="G24" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="24" t="s">
+      <c r="H24" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="I24" s="24" t="s">
+      <c r="I24" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="24"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="24"/>
-      <c r="Q24" s="24"/>
-      <c r="R24" s="24"/>
-      <c r="S24" s="24"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="28"/>
+      <c r="Q24" s="28"/>
+      <c r="R24" s="28"/>
+      <c r="S24" s="28"/>
       <c r="T24" s="3"/>
     </row>
     <row r="25" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
       <c r="I25" s="3" t="s">
         <v>51</v>
       </c>
@@ -3512,7 +3549,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H11"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3812,7 +3849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F20"/>
     </sheetView>
   </sheetViews>
@@ -4050,4 +4087,474 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:K21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1">
+        <v>6</v>
+      </c>
+      <c r="C1">
+        <v>6</v>
+      </c>
+      <c r="D1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <f>MMULT(B3:D3,F3:F5)</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="H4">
+        <f>MMULT(B4:D4,F3:F5)</f>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>7</v>
+      </c>
+      <c r="H5">
+        <f>MMULT(B5:D5,F3:F5)</f>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7">
+        <f>SUM(B1:D1)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8">
+        <f>AVERAGE(B1:D1)</f>
+        <v>6.333333333333333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9">
+        <f>_xlfn.MODE.SNGL(B1:D1)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10">
+        <f xml:space="preserve"> _xlfn.VAR.P(B1:D1)</f>
+        <v>0.22222222222222224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11">
+        <f xml:space="preserve"> MIN(B1:D1)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12">
+        <f>MAX(B1:D1)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="J14" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="K14" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="26">
+        <v>1</v>
+      </c>
+      <c r="B15" s="26">
+        <v>45</v>
+      </c>
+      <c r="C15" s="26">
+        <v>10</v>
+      </c>
+      <c r="D15" s="26">
+        <v>10</v>
+      </c>
+      <c r="E15" s="26">
+        <v>49</v>
+      </c>
+      <c r="F15" s="26">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G15" s="26">
+        <v>1</v>
+      </c>
+      <c r="H15" s="26">
+        <v>7.28</v>
+      </c>
+      <c r="I15" s="26">
+        <v>1</v>
+      </c>
+      <c r="J15" s="26">
+        <v>10</v>
+      </c>
+      <c r="K15" s="25">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="L15" s="26"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="26">
+        <v>2</v>
+      </c>
+      <c r="B16" s="26">
+        <v>45</v>
+      </c>
+      <c r="C16" s="26">
+        <v>100</v>
+      </c>
+      <c r="D16" s="26">
+        <v>100</v>
+      </c>
+      <c r="E16" s="26">
+        <v>540</v>
+      </c>
+      <c r="F16" s="26">
+        <v>5.4</v>
+      </c>
+      <c r="G16" s="26">
+        <v>6</v>
+      </c>
+      <c r="H16" s="26">
+        <v>7.7199970000000002</v>
+      </c>
+      <c r="I16" s="26">
+        <v>1</v>
+      </c>
+      <c r="J16" s="26">
+        <v>10</v>
+      </c>
+      <c r="K16" s="26">
+        <v>0.503</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="26">
+        <v>3</v>
+      </c>
+      <c r="B17" s="26">
+        <v>45</v>
+      </c>
+      <c r="C17" s="26">
+        <v>200</v>
+      </c>
+      <c r="D17" s="26">
+        <v>200</v>
+      </c>
+      <c r="E17" s="26">
+        <v>1064</v>
+      </c>
+      <c r="F17" s="26">
+        <v>5.32</v>
+      </c>
+      <c r="G17" s="26">
+        <v>5</v>
+      </c>
+      <c r="H17">
+        <v>8.0675860000000004</v>
+      </c>
+      <c r="I17" s="26">
+        <v>1</v>
+      </c>
+      <c r="J17" s="26">
+        <v>10</v>
+      </c>
+      <c r="K17" s="26">
+        <v>1.71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="26">
+        <v>4</v>
+      </c>
+      <c r="B18" s="26">
+        <v>45</v>
+      </c>
+      <c r="C18" s="26">
+        <v>300</v>
+      </c>
+      <c r="D18" s="26">
+        <v>300</v>
+      </c>
+      <c r="E18" s="26">
+        <v>1583</v>
+      </c>
+      <c r="F18" s="26">
+        <v>5.2766669999999998</v>
+      </c>
+      <c r="G18" s="26">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>8.2467790000000001</v>
+      </c>
+      <c r="I18" s="26">
+        <v>1</v>
+      </c>
+      <c r="J18" s="26">
+        <v>10</v>
+      </c>
+      <c r="K18" s="26">
+        <v>3.7120000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="26">
+        <v>5</v>
+      </c>
+      <c r="B19" s="26">
+        <v>45</v>
+      </c>
+      <c r="C19" s="26">
+        <v>500</v>
+      </c>
+      <c r="D19" s="26">
+        <v>500</v>
+      </c>
+      <c r="E19" s="26">
+        <v>2699</v>
+      </c>
+      <c r="F19" s="26">
+        <v>5.3979999999999997</v>
+      </c>
+      <c r="G19" s="26">
+        <v>5</v>
+      </c>
+      <c r="H19">
+        <v>8.4355919999999998</v>
+      </c>
+      <c r="I19" s="26">
+        <v>1</v>
+      </c>
+      <c r="J19" s="26">
+        <v>10</v>
+      </c>
+      <c r="K19" s="26">
+        <v>10.015000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="26">
+        <v>6</v>
+      </c>
+      <c r="B20" s="26">
+        <v>45</v>
+      </c>
+      <c r="C20" s="26">
+        <v>1000</v>
+      </c>
+      <c r="D20" s="26">
+        <v>500</v>
+      </c>
+      <c r="E20" s="26">
+        <v>2699</v>
+      </c>
+      <c r="F20" s="26">
+        <v>5.3979999999999997</v>
+      </c>
+      <c r="G20" s="26">
+        <v>5</v>
+      </c>
+      <c r="H20" s="26">
+        <v>8.4355919999999998</v>
+      </c>
+      <c r="I20" s="26">
+        <v>1</v>
+      </c>
+      <c r="J20" s="26">
+        <v>10</v>
+      </c>
+      <c r="K20" s="26">
+        <v>20.097999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="26">
+        <v>7</v>
+      </c>
+      <c r="B21" s="26">
+        <v>45</v>
+      </c>
+      <c r="C21" s="26">
+        <v>500</v>
+      </c>
+      <c r="D21" s="26">
+        <v>1000</v>
+      </c>
+      <c r="E21" s="26">
+        <v>5647</v>
+      </c>
+      <c r="F21" s="26">
+        <v>5.6470000000000002</v>
+      </c>
+      <c r="G21" s="26">
+        <v>8</v>
+      </c>
+      <c r="H21" s="26">
+        <v>8.3583599999999993</v>
+      </c>
+      <c r="I21" s="26">
+        <v>1</v>
+      </c>
+      <c r="J21" s="26">
+        <v>10</v>
+      </c>
+      <c r="K21" s="26">
+        <v>19.946999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="26">
+        <v>8</v>
+      </c>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="26">
+        <v>9</v>
+      </c>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="26">
+        <v>10</v>
+      </c>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>